<commit_message>
Uploaded 09-Apr-2021 16:54:46 {/src/main/resources/com/myspace/test/rules.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/test/rules.xlsx
+++ b/src/main/resources/com/myspace/test/rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA9E7491-47BE-44A1-9F36-34FFFB3D12AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{267950CE-C319-4301-A516-994E71E97753}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="259" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2552,7 +2552,7 @@
       <c r="L48" s="20"/>
       <c r="M48" s="25"/>
       <c r="N48" s="24" t="s">
-        <v>157</v>
+        <v>86</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Uploaded 12-Apr-2021 10:56:04 {/src/main/resources/com/myspace/test/rules.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/test/rules.xlsx
+++ b/src/main/resources/com/myspace/test/rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A670A7F7-2614-44DC-9FD6-25CAEA7AF594}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948A213A-C5A2-499C-9E7F-AA0BCAE9D147}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="259" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="169">
   <si>
     <t>RuleSet</t>
   </si>
@@ -531,9 +531,6 @@
   </si>
   <si>
     <t>com.myspace.test.Patient</t>
-  </si>
-  <si>
-    <t>General Followup(Ped follow up1)</t>
   </si>
 </sst>
 </file>
@@ -1218,10 +1215,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N1027"/>
+  <dimension ref="A1:N1026"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="I43" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="N48" sqref="N48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2555,20 +2552,14 @@
       <c r="L48" s="20"/>
       <c r="M48" s="25"/>
       <c r="N48" s="24" t="s">
-        <v>157</v>
+        <v>86</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A49" s="20" t="s">
-        <v>169</v>
-      </c>
+      <c r="A49" s="20"/>
       <c r="B49" s="28"/>
-      <c r="C49" s="28">
-        <v>18</v>
-      </c>
-      <c r="D49" s="21" t="s">
-        <v>92</v>
-      </c>
+      <c r="C49" s="28"/>
+      <c r="D49" s="21"/>
       <c r="E49" s="20"/>
       <c r="F49" s="34"/>
       <c r="G49" s="34"/>
@@ -2578,25 +2569,13 @@
       <c r="K49" s="20"/>
       <c r="L49" s="20"/>
       <c r="M49" s="25"/>
-      <c r="N49" s="24" t="s">
-        <v>157</v>
-      </c>
+      <c r="N49" s="24"/>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A50" s="20"/>
-      <c r="B50" s="28"/>
-      <c r="C50" s="28"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="34"/>
-      <c r="G50" s="34"/>
-      <c r="H50" s="20"/>
-      <c r="I50" s="20"/>
-      <c r="J50" s="20"/>
-      <c r="K50" s="20"/>
-      <c r="L50" s="20"/>
-      <c r="M50" s="25"/>
-      <c r="N50" s="24"/>
+      <c r="B50" s="29"/>
+      <c r="C50" s="31"/>
+      <c r="F50" s="35"/>
+      <c r="G50" s="35"/>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B51" s="29"/>
@@ -6747,8 +6726,6 @@
     <row r="742" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B742" s="29"/>
       <c r="C742" s="31"/>
-      <c r="F742" s="35"/>
-      <c r="G742" s="35"/>
     </row>
     <row r="743" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B743" s="29"/>
@@ -7072,7 +7049,6 @@
     </row>
     <row r="823" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B823" s="29"/>
-      <c r="C823" s="31"/>
     </row>
     <row r="824" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B824" s="29"/>
@@ -7682,9 +7658,6 @@
     </row>
     <row r="1026" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1026" s="29"/>
-    </row>
-    <row r="1027" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1027" s="29"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -7694,13 +7667,13 @@
     <mergeCell ref="B8:L8"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D11:D1121 M11:M876" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J50:J870 K50:K711 L11:L693 J11:K49" xr:uid="{00000000-0002-0000-0000-000001000000}">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D11:D1120 M11:M875" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"""Ancillary and Vaccination"",""Sick Visit"",""Pre-Op Clearance"",""Well Visit"",""General Follow Up"",""Adult Sick Visit"",""Medicare Sick Visit"",""Pediatric Sick Visit"",""Medicare Wellness Visit"",""Well Child Visit"",""Annual Physical Visit"""</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J51:J871 L11:L694 J11:K50 K51:K712" xr:uid="{00000000-0002-0000-0000-000001000000}">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F11:I50" xr:uid="{FDB25CDC-1A47-40E7-9CE9-F1E87EFBC655}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F11:I49" xr:uid="{FDB25CDC-1A47-40E7-9CE9-F1E87EFBC655}">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
@@ -7718,13 +7691,13 @@
           <x14:formula1>
             <xm:f>'Dropdown List'!$A$2:$A$55</xm:f>
           </x14:formula1>
-          <xm:sqref>E11:E933</xm:sqref>
+          <xm:sqref>E11:E932</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
             <xm:f>'Dropdown List'!$C$2:$C$35</xm:f>
           </x14:formula1>
-          <xm:sqref>N11:N901</xm:sqref>
+          <xm:sqref>N11:N900</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>